<commit_message>
Uploading DB with sample data
</commit_message>
<xml_diff>
--- a/RATMSWeb/sql_scripts/Script_tracker.xlsx
+++ b/RATMSWeb/sql_scripts/Script_tracker.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20353"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20354"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8843F8-0060-46FF-8E00-7486C478181D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5DEDA3-3F24-4905-894A-E49624CF73B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>SL NO</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Anson Antony</t>
+  </si>
+  <si>
+    <t>Dummy_Data</t>
   </si>
 </sst>
 </file>
@@ -358,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,25 +400,21 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="B4" t="s">
         <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>